<commit_message>
Updated report and excel data
</commit_message>
<xml_diff>
--- a/project1/report/data.xlsx
+++ b/project1/report/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joo Kai\Documents\GitHub\CITS5507-HPC\project1\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3278FFF-C776-4517-B63F-81AC4DDA479A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014C904C-797B-4698-A5E2-274D576BCDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5100" windowWidth="28110" windowHeight="16440" xr2:uid="{B4D0E340-C36E-4AD0-92A5-AA082ACFC92F}"/>
   </bookViews>
@@ -25,30 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>Num threads</t>
-  </si>
-  <si>
-    <t>Experiment 1</t>
-  </si>
-  <si>
-    <t>Experiment 2</t>
-  </si>
-  <si>
-    <t>Num fish</t>
-  </si>
-  <si>
-    <t>Trial 1</t>
-  </si>
-  <si>
-    <t>Experiment 3</t>
-  </si>
-  <si>
-    <t>Num Steps</t>
-  </si>
-  <si>
-    <t>Experiment 4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+  <si>
+    <t>Sequential</t>
   </si>
   <si>
     <t>Static</t>
@@ -60,25 +39,55 @@
     <t>Guided</t>
   </si>
   <si>
-    <t xml:space="preserve">Schedule </t>
-  </si>
-  <si>
-    <t>Experiment 5</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
     <t>Taskloop</t>
   </si>
   <si>
-    <t>Time (s)</t>
-  </si>
-  <si>
-    <t>Experiment 6</t>
-  </si>
-  <si>
     <t>Sections</t>
+  </si>
+  <si>
+    <t>exp1</t>
+  </si>
+  <si>
+    <t>exp1t</t>
+  </si>
+  <si>
+    <t>exp2</t>
+  </si>
+  <si>
+    <t>exp2t</t>
+  </si>
+  <si>
+    <t>exp3</t>
+  </si>
+  <si>
+    <t>exp3t</t>
+  </si>
+  <si>
+    <t>exp4</t>
+  </si>
+  <si>
+    <t>exp4t</t>
+  </si>
+  <si>
+    <t>exp5</t>
+  </si>
+  <si>
+    <t>exp5t</t>
+  </si>
+  <si>
+    <t>exp6</t>
+  </si>
+  <si>
+    <t>exp6t</t>
+  </si>
+  <si>
+    <t>Parallel Base</t>
+  </si>
+  <si>
+    <t>Runtime</t>
   </si>
 </sst>
 </file>
@@ -114,17 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,271 +443,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBD5FB5-7059-45C4-9A3D-052EE4658EE8}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>17.86571</v>
+      </c>
+      <c r="C2">
+        <v>5000</v>
+      </c>
+      <c r="D2">
+        <v>11.239551000000001</v>
+      </c>
+      <c r="E2">
+        <v>5000</v>
+      </c>
+      <c r="F2">
+        <v>10.163383</v>
+      </c>
+      <c r="G2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>17.86571</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>17.86571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>18.216635</v>
+      </c>
+      <c r="C3">
+        <v>10000</v>
+      </c>
+      <c r="D3">
+        <v>20.407219000000001</v>
+      </c>
+      <c r="E3">
+        <v>10000</v>
+      </c>
+      <c r="F3">
+        <v>20.238112000000001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>20.25028</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3">
+        <v>20.25028</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>18.514851</v>
+      </c>
+      <c r="C4">
+        <v>15000</v>
+      </c>
+      <c r="D4">
+        <v>29.593074999999999</v>
+      </c>
+      <c r="E4">
+        <v>15000</v>
+      </c>
+      <c r="F4">
+        <v>30.306684000000001</v>
+      </c>
+      <c r="G4" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>12.904030000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="H4">
+        <v>18.060746000000002</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>18.274405000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>19.101870000000002</v>
+      </c>
+      <c r="C5">
+        <v>20000</v>
+      </c>
+      <c r="D5">
+        <v>38.734811999999998</v>
+      </c>
+      <c r="E5">
+        <v>20000</v>
+      </c>
+      <c r="F5">
+        <v>40.372430000000001</v>
+      </c>
+      <c r="G5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>12.130501000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="H5">
+        <v>19.621511999999999</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>18.471405000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>20.25028</v>
+      </c>
+      <c r="C6">
+        <v>40000</v>
+      </c>
+      <c r="D6">
+        <v>75.324484999999996</v>
+      </c>
+      <c r="E6">
+        <v>40000</v>
+      </c>
+      <c r="F6">
+        <v>67.619606000000005</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>18.410658000000002</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>12.37898</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>12.896915</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>20.466868000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B7">
-        <v>13.902485</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22.50976</v>
+      </c>
+      <c r="C7">
+        <v>60000</v>
+      </c>
+      <c r="D7">
+        <v>111.749207</v>
+      </c>
+      <c r="E7">
+        <v>60000</v>
+      </c>
+      <c r="F7">
+        <v>94.011695000000003</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>19.779443000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B8">
-        <v>15.860992</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5000</v>
-      </c>
-      <c r="B11">
-        <v>7.8766970000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10000</v>
-      </c>
-      <c r="B12">
-        <v>13.971674</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>15000</v>
-      </c>
-      <c r="B13">
-        <v>20.067333000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>20000</v>
-      </c>
-      <c r="B14">
-        <v>26.154729</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>25000</v>
-      </c>
-      <c r="B15">
-        <v>32.223322000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>5000</v>
-      </c>
-      <c r="B18">
-        <v>7.0449489999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>10000</v>
-      </c>
-      <c r="B19">
-        <v>14.037083000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>15000</v>
-      </c>
-      <c r="B20">
-        <v>21.025368</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20000</v>
-      </c>
-      <c r="B21">
-        <v>28.018678000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>25000</v>
-      </c>
-      <c r="B22">
-        <v>35.012374999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25">
-        <v>14.164837</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26">
-        <v>15.469175</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27">
-        <v>14.531245999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29">
-        <v>14.561199999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30">
-        <v>20.832470000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32">
-        <v>14.017635</v>
+        <v>27.131281000000001</v>
+      </c>
+      <c r="C8">
+        <v>80000</v>
+      </c>
+      <c r="D8">
+        <v>148.04376199999999</v>
+      </c>
+      <c r="E8">
+        <v>80000</v>
+      </c>
+      <c r="F8">
+        <v>111.352626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>100000</v>
+      </c>
+      <c r="D9">
+        <v>184.47862900000001</v>
+      </c>
+      <c r="E9">
+        <v>100000</v>
+      </c>
+      <c r="F9">
+        <v>130.86227199999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A28:B28"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Report first draft fully complete
</commit_message>
<xml_diff>
--- a/project1/report/data.xlsx
+++ b/project1/report/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joo Kai\Documents\GitHub\CITS5507-HPC\project1\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014C904C-797B-4698-A5E2-274D576BCDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B43812D-66AB-4879-B57B-272FAB2C263C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5100" windowWidth="28110" windowHeight="16440" xr2:uid="{B4D0E340-C36E-4AD0-92A5-AA082ACFC92F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Sequential</t>
   </si>
@@ -78,16 +78,25 @@
     <t>exp5t</t>
   </si>
   <si>
-    <t>exp6</t>
-  </si>
-  <si>
-    <t>exp6t</t>
-  </si>
-  <si>
     <t>Parallel Base</t>
   </si>
   <si>
     <t>Runtime</t>
+  </si>
+  <si>
+    <t>exp0</t>
+  </si>
+  <si>
+    <t>exp0t</t>
+  </si>
+  <si>
+    <t>SequentialOld</t>
+  </si>
+  <si>
+    <t>ParallelOld</t>
+  </si>
+  <si>
+    <t>Parallel</t>
   </si>
 </sst>
 </file>
@@ -123,12 +132,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,282 +453,306 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBD5FB5-7059-45C4-9A3D-052EE4658EE8}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>15.709291</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>17.86571</v>
-      </c>
-      <c r="C2">
-        <v>5000</v>
-      </c>
       <c r="D2">
-        <v>11.239551000000001</v>
+        <v>15.709291</v>
       </c>
       <c r="E2">
         <v>5000</v>
       </c>
       <c r="F2">
-        <v>10.163383</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
+        <v>8.4488120000000002</v>
+      </c>
+      <c r="G2">
+        <v>5000</v>
       </c>
       <c r="H2">
-        <v>17.86571</v>
+        <v>8.3470510000000004</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>17.86571</v>
+        <v>15.709291</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>15.709291</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>15.928094</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>18.216635</v>
-      </c>
-      <c r="C3">
-        <v>10000</v>
-      </c>
       <c r="D3">
-        <v>20.407219000000001</v>
+        <v>16.295912000000001</v>
       </c>
       <c r="E3">
         <v>10000</v>
       </c>
       <c r="F3">
-        <v>20.238112000000001</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
+        <v>16.607592</v>
+      </c>
+      <c r="G3">
+        <v>10000</v>
       </c>
       <c r="H3">
-        <v>20.25028</v>
+        <v>16.607037999999999</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J3">
-        <v>20.25028</v>
+        <v>16.536090000000002</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3">
+        <v>16.536090000000002</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>16.536090000000002</v>
+      </c>
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>18.514851</v>
-      </c>
-      <c r="C4">
-        <v>15000</v>
-      </c>
       <c r="D4">
-        <v>29.593074999999999</v>
+        <v>16.559909000000001</v>
       </c>
       <c r="E4">
         <v>15000</v>
       </c>
       <c r="F4">
-        <v>30.306684000000001</v>
-      </c>
-      <c r="G4" t="s">
+        <v>24.701730000000001</v>
+      </c>
+      <c r="G4">
+        <v>15000</v>
+      </c>
+      <c r="H4">
+        <v>24.857468000000001</v>
+      </c>
+      <c r="I4" t="s">
         <v>1</v>
       </c>
-      <c r="H4">
-        <v>18.060746000000002</v>
-      </c>
-      <c r="I4" t="s">
-        <v>6</v>
-      </c>
       <c r="J4">
-        <v>18.274405000000002</v>
+        <v>16.490687000000001</v>
+      </c>
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>17.043983000000001</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>16.557117000000002</v>
+      </c>
+      <c r="C5">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>19.101870000000002</v>
-      </c>
-      <c r="C5">
-        <v>20000</v>
-      </c>
       <c r="D5">
-        <v>38.734811999999998</v>
+        <v>17.114429999999999</v>
       </c>
       <c r="E5">
         <v>20000</v>
       </c>
       <c r="F5">
-        <v>40.372430000000001</v>
-      </c>
-      <c r="G5" t="s">
+        <v>32.786861999999999</v>
+      </c>
+      <c r="G5">
+        <v>20000</v>
+      </c>
+      <c r="H5">
+        <v>33.108902</v>
+      </c>
+      <c r="I5" t="s">
         <v>2</v>
       </c>
-      <c r="H5">
-        <v>19.621511999999999</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
       <c r="J5">
-        <v>18.471405000000001</v>
+        <v>17.747706000000001</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>17.838336999999999</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C6">
         <v>16</v>
       </c>
-      <c r="B6">
-        <v>20.25028</v>
-      </c>
-      <c r="C6">
-        <v>40000</v>
-      </c>
       <c r="D6">
-        <v>75.324484999999996</v>
+        <v>18.140611</v>
       </c>
       <c r="E6">
         <v>40000</v>
       </c>
       <c r="F6">
-        <v>67.619606000000005</v>
-      </c>
-      <c r="G6" t="s">
+        <v>65.250904000000006</v>
+      </c>
+      <c r="G6">
+        <v>40000</v>
+      </c>
+      <c r="H6">
+        <v>54.529052999999998</v>
+      </c>
+      <c r="I6" t="s">
         <v>3</v>
       </c>
-      <c r="H6">
-        <v>18.410658000000002</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="J6">
-        <v>20.466868000000002</v>
+        <v>16.550087000000001</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <v>17.87425</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="C7">
         <v>32</v>
       </c>
-      <c r="B7">
-        <v>22.50976</v>
-      </c>
-      <c r="C7">
-        <v>60000</v>
-      </c>
       <c r="D7">
-        <v>111.749207</v>
+        <v>20.400532999999999</v>
       </c>
       <c r="E7">
         <v>60000</v>
       </c>
       <c r="F7">
-        <v>94.011695000000003</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
+        <v>97.634416999999999</v>
+      </c>
+      <c r="G7">
+        <v>60000</v>
       </c>
       <c r="H7">
-        <v>19.779443000000001</v>
+        <v>75.213846000000004</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7">
+        <v>17.904565999999999</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C8">
         <v>64</v>
       </c>
-      <c r="B8">
-        <v>27.131281000000001</v>
-      </c>
-      <c r="C8">
-        <v>80000</v>
-      </c>
       <c r="D8">
-        <v>148.04376199999999</v>
+        <v>24.238047000000002</v>
       </c>
       <c r="E8">
         <v>80000</v>
       </c>
       <c r="F8">
-        <v>111.352626</v>
+        <v>130.061722</v>
+      </c>
+      <c r="G8">
+        <v>80000</v>
+      </c>
+      <c r="H8">
+        <v>95.886895999999993</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>100000</v>
-      </c>
-      <c r="D9">
-        <v>184.47862900000001</v>
-      </c>
       <c r="E9">
         <v>100000</v>
       </c>
       <c r="F9">
-        <v>130.86227199999999</v>
+        <v>162.498987</v>
+      </c>
+      <c r="G9">
+        <v>100000</v>
+      </c>
+      <c r="H9">
+        <v>116.609549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report updated to include chunks
</commit_message>
<xml_diff>
--- a/project1/report/data.xlsx
+++ b/project1/report/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joo Kai\Documents\GitHub\CITS5507-HPC\project1\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B43812D-66AB-4879-B57B-272FAB2C263C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9EEBFB-D6FE-4702-A8BB-8E867EA4B789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="5100" windowWidth="28110" windowHeight="16440" xr2:uid="{B4D0E340-C36E-4AD0-92A5-AA082ACFC92F}"/>
+    <workbookView xWindow="-27990" yWindow="5010" windowWidth="28110" windowHeight="16440" xr2:uid="{B4D0E340-C36E-4AD0-92A5-AA082ACFC92F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,13 +90,13 @@
     <t>exp0t</t>
   </si>
   <si>
-    <t>SequentialOld</t>
-  </si>
-  <si>
-    <t>ParallelOld</t>
-  </si>
-  <si>
     <t>Parallel</t>
+  </si>
+  <si>
+    <t>SequentialCondensed</t>
+  </si>
+  <si>
+    <t>ParallelCondensed</t>
   </si>
 </sst>
 </file>
@@ -454,12 +454,12 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -513,7 +513,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>15.709291</v>
@@ -551,10 +551,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>15.928094</v>
+        <v>16.116607999999999</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>16.536090000000002</v>

</xml_diff>